<commit_message>
Final hardware update and first software beginning
We have finished the hardware design of the machine, and tested successfully. And now, we focus on the software building.
</commit_message>
<xml_diff>
--- a/DownFormat.xlsx
+++ b/DownFormat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emb\B1ROV\OurEDA-B1S\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Emb\B1ROV\OurEDA-B1S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA68B33-77CB-4A8A-970A-93A2D642BEC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B31366-971B-4533-9195-B621AE228543}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="3390" windowWidth="20640" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4730" yWindow="5020" windowWidth="18500" windowHeight="10510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>起始位</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,26 +43,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>侧推开关</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>定向开关</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>定深开关</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>推进模式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>姿态调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>结束位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,23 +93,41 @@
   <si>
     <t>PWM10</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定向定深侧推</t>
+  </si>
+  <si>
+    <t>侧推+1</t>
+  </si>
+  <si>
+    <t>定向+2</t>
+  </si>
+  <si>
+    <t>定深+4</t>
+  </si>
+  <si>
+    <t>模式开关</t>
+  </si>
+  <si>
+    <t>验证位</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -143,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -166,19 +164,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -459,231 +494,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC1:AF3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="S1" s="3"/>
+      <c r="T1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="7"/>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="8"/>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2">
+        <v>9</v>
+      </c>
+      <c r="K3" s="2">
+        <v>10</v>
+      </c>
+      <c r="L3" s="2">
+        <v>11</v>
+      </c>
+      <c r="M3" s="2">
+        <v>12</v>
+      </c>
+      <c r="N3" s="2">
+        <v>13</v>
+      </c>
+      <c r="O3" s="2">
+        <v>14</v>
+      </c>
+      <c r="P3" s="2">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>16</v>
+      </c>
+      <c r="R3" s="2">
         <v>17</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2" t="s">
+      <c r="S3" s="2">
         <v>18</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2" t="s">
+      <c r="T3" s="2">
         <v>19</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2" t="s">
+      <c r="U3" s="2">
         <v>20</v>
       </c>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2" t="s">
+      <c r="V3" s="2">
         <v>21</v>
       </c>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="W3" s="2">
+        <v>22</v>
+      </c>
+      <c r="X3" s="2">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>27</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>29</v>
+      </c>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="8"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3" t="s">
-        <v>11</v>
-      </c>
+    <row r="5" spans="1:32">
+      <c r="AB5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3">
-        <v>7</v>
-      </c>
-      <c r="I3" s="3">
-        <v>8</v>
-      </c>
-      <c r="J3" s="3">
-        <v>9</v>
-      </c>
-      <c r="K3" s="3">
-        <v>10</v>
-      </c>
-      <c r="L3" s="3">
-        <v>11</v>
-      </c>
-      <c r="M3" s="3">
-        <v>12</v>
-      </c>
-      <c r="N3" s="3">
-        <v>13</v>
-      </c>
-      <c r="O3" s="3">
-        <v>14</v>
-      </c>
-      <c r="P3" s="3">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>16</v>
-      </c>
-      <c r="R3" s="3">
-        <v>17</v>
-      </c>
-      <c r="S3" s="3">
+    <row r="6" spans="1:32">
+      <c r="AB6" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="3">
+      <c r="AC6" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="3">
+      <c r="AD6" t="s">
         <v>20</v>
-      </c>
-      <c r="V3" s="3">
-        <v>21</v>
-      </c>
-      <c r="W3" s="3">
-        <v>22</v>
-      </c>
-      <c r="X3" s="3">
-        <v>23</v>
-      </c>
-      <c r="Y3" s="3">
-        <v>24</v>
-      </c>
-      <c r="Z3" s="3">
-        <v>25</v>
-      </c>
-      <c r="AA3" s="3">
-        <v>26</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>27</v>
-      </c>
-      <c r="AC3" s="3">
-        <v>28</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>29</v>
-      </c>
-      <c r="AE3" s="3">
-        <v>30</v>
-      </c>
-      <c r="AF3" s="3">
-        <v>31</v>
-      </c>
-      <c r="AG3" s="3">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="AB5:AD5"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
@@ -691,12 +730,12 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update ROVlibs and layout Debugs
</commit_message>
<xml_diff>
--- a/DownFormat.xlsx
+++ b/DownFormat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git_repository\OurEDA\OurEDA-B1S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60730B2-B7BB-457B-8C26-F49EDE30AA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229F7AB9-37CC-406A-8838-37212B0782BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t>起始位</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,7 +154,151 @@
     <t>继电器+8</t>
   </si>
   <si>
-    <t>2506D606D606D606D606D606D605DC05DC05DC05DC05DC05DC0000000021</t>
+    <t>前进</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模式选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定向模式开关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>继电器开关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定深模式开关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>侧推模式开关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推进器稳定，灯光稳定，云台不动，传送带不动，机械臂不动，开启继电器，关闭侧推模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2505DC05DC05DC05DC05DC05DC0000000000000000000000000000080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推进器稳定，灯光稳定，云台不动，传送带不动，机械臂不动，关闭继电器，关闭侧推模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2505DC05DC05DC05DC05DC05DC0000000000000000000000000000000021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试实例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后退</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2507D005DC05DC05DC05DC05DC0000000000000000000000000000080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2503E805DC05DC05DC05DC05DC0000000000000000000000000000080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开启侧推</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前进+左转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前进+右转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2507D007D005DC05DC05DC05DC0000000000000000000000000000090021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2507D003E805DC05DC05DC05DC0000000000000000000000000000090021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械臂1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械臂2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械臂3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械臂4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械臂5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2505DC05DC05DC05DC05DC05DC05DC000000000000000000000000080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2505DC05DC05DC05DC05DC05DC000005DC00000000000000000000080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2505DC05DC05DC05DC05DC05DC0000000005DC0000000000000000080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2505DC05DC05DC05DC05DC05DC00000000000005DC000000000000080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2505DC05DC05DC05DC05DC05DC000000000000000005DC00000000080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2505DC05DC05DC05DC05DC09C40000000000000000000000000000080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2505DC05DC05DC05DC05DC05DC0000000000000000000001F401F4080021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>传送带满转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 预留引脚PWM最小</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -248,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -272,6 +416,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,12 +431,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -567,70 +713,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AF45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14" t="s">
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14" t="s">
+      <c r="S1" s="13"/>
+      <c r="T1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14" t="s">
+      <c r="U1" s="13"/>
+      <c r="V1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14" t="s">
+      <c r="W1" s="13"/>
+      <c r="X1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14" t="s">
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AA1" s="14"/>
+      <c r="AA1" s="13"/>
       <c r="AB1" s="1" t="s">
         <v>11</v>
       </c>
@@ -647,58 +796,58 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="W2" s="12"/>
-      <c r="X2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA2" s="12"/>
+      <c r="B2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="16"/>
+      <c r="P2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="16"/>
+      <c r="T2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="16"/>
+      <c r="V2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="16"/>
+      <c r="X2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA2" s="16"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="5" t="s">
@@ -802,17 +951,23 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA5" s="13" t="s">
+      <c r="U5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U6" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="AA6" t="s">
         <v>8</v>
       </c>
@@ -826,11 +981,33 @@
         <v>39</v>
       </c>
     </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U7" t="s">
+        <v>43</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U8" t="s">
+        <v>44</v>
+      </c>
+      <c r="V8" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="Y9" s="14" t="s">
+      <c r="U9" t="s">
+        <v>45</v>
+      </c>
+      <c r="V9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="Z9" s="14"/>
+      <c r="Z9" s="13"/>
       <c r="AA9" s="2" t="s">
         <v>27</v>
       </c>
@@ -845,10 +1022,11 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="Y10" s="14" t="s">
+      <c r="A10" s="11"/>
+      <c r="Y10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Z10" s="14"/>
+      <c r="Z10" s="13"/>
       <c r="AA10" s="2">
         <v>12</v>
       </c>
@@ -866,14 +1044,14 @@
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="13"/>
       <c r="F13" s="3" t="s">
         <v>11</v>
       </c>
@@ -888,14 +1066,14 @@
       <c r="A14" s="3">
         <v>0</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="10" t="s">
         <v>19</v>
       </c>
@@ -906,12 +1084,175 @@
         <v>21</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
@@ -919,28 +1260,6 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>